<commit_message>
Añadidos apartados a la memoria y modificada la matriz de estrategias
</commit_message>
<xml_diff>
--- a/Repositorio/Proyecto/DocumentosPropios/MatrizGestionInteresados.xlsx
+++ b/Repositorio/Proyecto/DocumentosPropios/MatrizGestionInteresados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\GitHub\PracticaXesPro_GrupoL\Repositorio\Proyecto\DocumentosPropios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergy6rey\Documents\GitHub\PracticaXesPro_GrupoL\Repositorio\Proyecto\DocumentosPropios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{14694691-CE12-4C12-9CD0-6EECA8C05A3F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{50FCF4C7-29B3-4E6A-B9CE-A3207D87556E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -986,7 +986,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,10 +994,10 @@
     <col min="1" max="2" width="22.21875" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>31</v>
       </c>

</xml_diff>